<commit_message>
Update models.xlsx to reflect models created and predictions made.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -20,150 +20,294 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
-  <si>
-    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="133">
+  <si>
+    <t>Hypers(ell=12.382259384067231)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SEStructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=9.9999999999544897e-06)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=7.1857373549553616)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Predicted?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>in progress</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saved?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEHamming 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_ML</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOO_log_P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tau</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hypers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.61996032729502459, var_p=2.1662971850616142)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=10.650074709352918)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.85864081521951263, var_p=0.33887648864814679)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>log_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.42482504515418229, var_p=0.77190328932157526)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>log_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.31273769260395001, var_p=0.78982392252858546)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell=19.200787723437394)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.43216924708580134, sigma_f=0.75326118251964591, ell=11.123560434547556)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.36174810262344692, ell=16.976484047437637)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.38187830426922176, ell0=783.32684463439443, ell1=15.804026532359993)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure SEHamming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell=18.06351933648082)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell=12.000240475426962)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.3738269324488715, sigma_f0=2.2901085164636997e-05, ell0=0.9232144412448956, sigma_f1=0.89026062827676122, ell1=8.5976136240155547)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -176,331 +320,247 @@
       </rPr>
       <t>atio</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=9.9999999999544897e-06)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(ell=13.714166977039794)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(ell=13.806560227522164)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(ell=13.2591061318578)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_p=5.1745145599243729)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(ell=13.306826612517378)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(sigma_f=6.2890530935004696, ell=18.586777104815493)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>bin_intensity_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(sigma_f=3.8457792489312168, ell=17.611476049271985)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.18673420272755697, ell0=184.17411469863069, ell1=14.14952382022827, var_p0=1.0000000000000001e-05)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>32Structure 52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.18655586807239488, ell0=184.48405585006759, ell1=14.145790499076451)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">52Structure </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>mKate_mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.34846026420753662, ell=28.741286142106219)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.33623853006661136, ell=32.060321150982823)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>mKate_mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.35483375851541427, sigma_f=0.93171412929598607, ell=21.939841462467648)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.35945193551611304, ell0=39.160914149618925, ell1=56.429026505115033)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>52Structure SEStructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>mKate_mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hypers(var_n=0.30307552926252879, ell0=28.741711216374707, sigma_f0=0.21305261382994262, ell1=0.90717603784446266)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>hamming SEStructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>mKate_mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SEStructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEHamming 52Structure structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kernel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_ML</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOO_log_P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tau</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hypers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.61996032729502459, var_p=2.1662971850616142)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=10.650074709352918)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=7.1857373549553616)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>sum_ratio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.85864081521951263, var_p=0.33887648864814679)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.42482504515418229, var_p=0.77190328932157526)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.31273769260395001, var_p=0.78982392252858546)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell=19.200787723437394)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.43216924708580134, sigma_f=0.75326118251964591, ell=11.123560434547556)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>52Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell=18.06351933648082)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell=12.000240475426962)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell=12.382259384067231)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.36174810262344692, ell=16.976484047437637)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.38187830426922176, ell0=783.32684463439443, ell1=15.804026532359993)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure 32Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure SEHamming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -513,7 +573,16 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -547,8 +616,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,10 +950,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -890,89 +961,113 @@
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
         <v>-104.296829</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.99829999999999997</v>
       </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3">
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>-107.403991</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.98550000000000004</v>
       </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4">
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
         <v>-109.175516</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.96719999999999995</v>
       </c>
-      <c r="H4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>-109.63411600000001</v>
@@ -981,32 +1076,44 @@
         <v>0.97330000000000005</v>
       </c>
       <c r="H5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
         <v>-115.755686</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.5242</v>
       </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C7">
         <v>-90.516735999999995</v>
@@ -1015,15 +1122,21 @@
         <v>0.99429999999999996</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>-95.730936999999997</v>
@@ -1032,15 +1145,21 @@
         <v>0.95009999999999994</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>-96.168786999999995</v>
@@ -1049,15 +1168,21 @@
         <v>0.95469999999999999</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>76</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C10">
         <v>-99.691761999999997</v>
@@ -1066,66 +1191,90 @@
         <v>0.86580000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11">
+        <v>78</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
         <v>-85.655743000000001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.93230000000000002</v>
       </c>
-      <c r="H11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12">
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
         <v>-85.967275999999998</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.96099999999999997</v>
       </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13">
+      <c r="H12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2">
         <v>-90.150796</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>0.94389999999999996</v>
       </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="C14">
         <v>-93.403767999999999</v>
@@ -1134,15 +1283,21 @@
         <v>0.92789999999999995</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <v>-94.193860000000001</v>
@@ -1151,15 +1306,21 @@
         <v>0.93010000000000004</v>
       </c>
       <c r="H15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>66</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C16">
         <v>-86.014349999999993</v>
@@ -1168,15 +1329,21 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>83</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>-95.681375000000003</v>
@@ -1185,15 +1352,21 @@
         <v>0.9768</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>77</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>-96.199038000000002</v>
@@ -1202,15 +1375,21 @@
         <v>0.98060000000000003</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>74</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C19">
         <v>-100.18935999999999</v>
@@ -1219,15 +1398,21 @@
         <v>0.91359999999999997</v>
       </c>
       <c r="H19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>55</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="C20">
         <v>-187.46480099999999</v>
@@ -1242,15 +1427,21 @@
         <v>0.45169999999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>106</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C21">
         <v>-188.51542900000001</v>
@@ -1265,15 +1456,21 @@
         <v>0.46039999999999998</v>
       </c>
       <c r="H21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <v>-188.611998</v>
@@ -1288,15 +1485,21 @@
         <v>0.45960000000000001</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>126</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="C23">
         <v>-189.126045</v>
@@ -1311,15 +1514,21 @@
         <v>0.4602</v>
       </c>
       <c r="H23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>103</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="C24">
         <v>-204.32833099999999</v>
@@ -1334,15 +1543,21 @@
         <v>0.22839999999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>119</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>-182.15376599999999</v>
@@ -1357,15 +1572,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>-182.15387799999999</v>
@@ -1380,38 +1601,50 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27">
+        <v>38</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="2" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
         <v>-182.15550500000001</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>-164.63807199999999</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>0.70020000000000004</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>0.5161</v>
       </c>
-      <c r="H27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C28">
         <v>-182.15568300000001</v>
@@ -1426,15 +1659,21 @@
         <v>0.5161</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>36</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>-182.38603000000001</v>
@@ -1449,15 +1688,21 @@
         <v>0.51190000000000002</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <v>-182.52230900000001</v>
@@ -1472,15 +1717,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C31">
         <v>-182.52231499999999</v>
@@ -1495,15 +1746,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>86</v>
+      </c>
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>-203.77469500000001</v>
@@ -1518,38 +1775,50 @@
         <v>0.35139999999999999</v>
       </c>
       <c r="H32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33">
+        <v>53</v>
+      </c>
+      <c r="I32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1">
+      <c r="A33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2">
         <v>-149.854615</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>-139.42251999999999</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>0.77890000000000004</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>0.57420000000000004</v>
       </c>
-      <c r="H33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="H33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="C34">
         <v>-150.395522</v>
@@ -1564,15 +1833,21 @@
         <v>0.57089999999999996</v>
       </c>
       <c r="H34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>109</v>
+      </c>
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <v>-150.76389699999999</v>
@@ -1587,38 +1862,50 @@
         <v>0.5696</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36">
+        <v>112</v>
+      </c>
+      <c r="I35" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2">
         <v>-150.853938</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>-139.5686</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>0.77990000000000004</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>0.56789999999999996</v>
       </c>
-      <c r="H36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="H36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
         <v>110</v>
-      </c>
-      <c r="B37" t="s">
-        <v>7</v>
       </c>
       <c r="C37">
         <v>-151.265311</v>
@@ -1633,15 +1920,21 @@
         <v>0.56659999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>111</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="C38">
         <v>-166.89236399999999</v>
@@ -1656,15 +1949,21 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>94</v>
+      </c>
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="C39">
         <v>-167.263352</v>
@@ -1679,15 +1978,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>99</v>
+      </c>
+      <c r="I39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>-167.263441</v>
@@ -1702,15 +2007,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>91</v>
+      </c>
+      <c r="I40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C41">
         <v>-167.358092</v>
@@ -1725,15 +2036,21 @@
         <v>0.56479999999999997</v>
       </c>
       <c r="H41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>71</v>
+      </c>
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C42">
         <v>-167.47835000000001</v>
@@ -1748,15 +2065,21 @@
         <v>0.56850000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>96</v>
+      </c>
+      <c r="I42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C43">
         <v>-167.644937</v>
@@ -1771,15 +2094,21 @@
         <v>0.56569999999999998</v>
       </c>
       <c r="H43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>92</v>
+      </c>
+      <c r="I43" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="C44">
         <v>-167.81095999999999</v>
@@ -1794,15 +2123,21 @@
         <v>0.56979999999999997</v>
       </c>
       <c r="H44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>61</v>
+      </c>
+      <c r="I44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C45">
         <v>-168.47959399999999</v>
@@ -1817,15 +2152,21 @@
         <v>0.55820000000000003</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>131</v>
+      </c>
+      <c r="I45" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="C46">
         <v>-192.916416</v>
@@ -1840,15 +2181,21 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>123</v>
+      </c>
+      <c r="I46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="C47">
         <v>-193.712221</v>
@@ -1863,15 +2210,21 @@
         <v>0.45739999999999997</v>
       </c>
       <c r="H47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>114</v>
+      </c>
+      <c r="I47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C48">
         <v>-193.892056</v>
@@ -1886,15 +2239,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>117</v>
+      </c>
+      <c r="I48" t="s">
+        <v>26</v>
+      </c>
+      <c r="J48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="C49">
         <v>-194.433592</v>
@@ -1909,15 +2268,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>127</v>
+      </c>
+      <c r="I49" t="s">
+        <v>26</v>
+      </c>
+      <c r="J49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C50">
         <v>-207.70643999999999</v>
@@ -1932,7 +2297,13 @@
         <v>0.18859999999999999</v>
       </c>
       <c r="H50" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="I50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +2311,7 @@
     <sortCondition ref="B3:B1048576"/>
     <sortCondition descending="1" ref="C3:C1048576"/>
   </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1964,36 +2335,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>-148.93375</v>
@@ -2008,11 +2379,12 @@
         <v>0.57379999999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Update models.xlsx to reflect models used to make predictions.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
   <si>
     <t>Hypers(ell=12.382259384067231)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -102,10 +102,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>in progress</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Saved?</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -122,10 +118,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">No </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -151,6 +143,18 @@
   </si>
   <si>
     <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>In progress</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -952,8 +956,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -963,34 +967,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
@@ -1010,10 +1014,10 @@
         <v>9</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1">
@@ -1033,10 +1037,10 @@
         <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1">
@@ -1053,21 +1057,21 @@
         <v>0.96719999999999995</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>-109.63411600000001</v>
@@ -1079,10 +1083,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1">
@@ -1102,18 +1106,18 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>-90.516735999999995</v>
@@ -1122,21 +1126,21 @@
         <v>0.99429999999999996</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>-95.730936999999997</v>
@@ -1145,21 +1149,21 @@
         <v>0.95009999999999994</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C9">
         <v>-96.168786999999995</v>
@@ -1168,21 +1172,21 @@
         <v>0.95469999999999999</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10">
         <v>-99.691761999999997</v>
@@ -1191,13 +1195,13 @@
         <v>0.86580000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1">
@@ -1217,10 +1221,10 @@
         <v>16</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1">
@@ -1237,13 +1241,13 @@
         <v>0.96099999999999997</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1">
@@ -1263,18 +1267,18 @@
         <v>18</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>-93.403767999999999</v>
@@ -1283,21 +1287,21 @@
         <v>0.92789999999999995</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <v>-94.193860000000001</v>
@@ -1306,21 +1310,21 @@
         <v>0.93010000000000004</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16">
         <v>-86.014349999999993</v>
@@ -1329,21 +1333,21 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>-95.681375000000003</v>
@@ -1352,21 +1356,21 @@
         <v>0.9768</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18">
         <v>-96.199038000000002</v>
@@ -1375,21 +1379,21 @@
         <v>0.98060000000000003</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>-100.18935999999999</v>
@@ -1398,21 +1402,21 @@
         <v>0.91359999999999997</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C20">
         <v>-187.46480099999999</v>
@@ -1427,21 +1431,21 @@
         <v>0.45169999999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C21">
         <v>-188.51542900000001</v>
@@ -1456,21 +1460,21 @@
         <v>0.46039999999999998</v>
       </c>
       <c r="H21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22">
         <v>-188.611998</v>
@@ -1485,21 +1489,21 @@
         <v>0.45960000000000001</v>
       </c>
       <c r="H22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C23">
         <v>-189.126045</v>
@@ -1514,21 +1518,21 @@
         <v>0.4602</v>
       </c>
       <c r="H23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C24">
         <v>-204.32833099999999</v>
@@ -1543,21 +1547,21 @@
         <v>0.22839999999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25">
         <v>-182.15376599999999</v>
@@ -1572,21 +1576,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26">
         <v>-182.15387799999999</v>
@@ -1601,13 +1605,13 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1">
@@ -1633,18 +1637,18 @@
         <v>6</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C28">
         <v>-182.15568300000001</v>
@@ -1659,21 +1663,21 @@
         <v>0.5161</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>-182.38603000000001</v>
@@ -1688,21 +1692,21 @@
         <v>0.51190000000000002</v>
       </c>
       <c r="H29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30">
         <v>-182.52230900000001</v>
@@ -1717,21 +1721,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>-182.52231499999999</v>
@@ -1746,21 +1750,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C32">
         <v>-203.77469500000001</v>
@@ -1775,13 +1779,13 @@
         <v>0.35139999999999999</v>
       </c>
       <c r="H32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1">
@@ -1804,21 +1808,21 @@
         <v>0.57420000000000004</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C34">
         <v>-150.395522</v>
@@ -1833,21 +1837,21 @@
         <v>0.57089999999999996</v>
       </c>
       <c r="H34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>-150.76389699999999</v>
@@ -1862,13 +1866,13 @@
         <v>0.5696</v>
       </c>
       <c r="H35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1">
@@ -1891,21 +1895,21 @@
         <v>0.56789999999999996</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C37">
         <v>-151.265311</v>
@@ -1920,21 +1924,21 @@
         <v>0.56659999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C38">
         <v>-166.89236399999999</v>
@@ -1949,21 +1953,21 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C39">
         <v>-167.263352</v>
@@ -1978,21 +1982,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H39" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C40">
         <v>-167.263441</v>
@@ -2007,21 +2011,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41">
         <v>-167.358092</v>
@@ -2036,21 +2040,21 @@
         <v>0.56479999999999997</v>
       </c>
       <c r="H41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42">
         <v>-167.47835000000001</v>
@@ -2065,21 +2069,21 @@
         <v>0.56850000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C43">
         <v>-167.644937</v>
@@ -2094,21 +2098,21 @@
         <v>0.56569999999999998</v>
       </c>
       <c r="H43" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C44">
         <v>-167.81095999999999</v>
@@ -2123,21 +2127,21 @@
         <v>0.56979999999999997</v>
       </c>
       <c r="H44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45">
         <v>-168.47959399999999</v>
@@ -2152,21 +2156,21 @@
         <v>0.55820000000000003</v>
       </c>
       <c r="H45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C46">
         <v>-192.916416</v>
@@ -2181,21 +2185,21 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C47">
         <v>-193.712221</v>
@@ -2210,21 +2214,21 @@
         <v>0.45739999999999997</v>
       </c>
       <c r="H47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48">
         <v>-193.892056</v>
@@ -2239,21 +2243,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I48" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J48" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49">
         <v>-194.433592</v>
@@ -2268,21 +2272,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50">
         <v>-207.70643999999999</v>
@@ -2297,16 +2301,17 @@
         <v>0.18859999999999999</v>
       </c>
       <c r="H50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="B3:B1048576"/>
     <sortCondition descending="1" ref="C3:C1048576"/>
@@ -2335,36 +2340,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>-148.93375</v>
@@ -2379,7 +2384,7 @@
         <v>0.57379999999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More models have been used for prediction.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -20,13 +20,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="134">
-  <si>
-    <t>Hypers(ell=12.382259384067231)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="135">
+  <si>
+    <t xml:space="preserve">52Structure 32Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure SEHamming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.33623853006661136, ell=32.060321150982823)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35483375851541427, sigma_f=0.93171412929598607, ell=21.939841462467648)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure 32Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35945193551611304, ell0=39.160914149618925, ell1=56.429026505115033)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.30307552926252879, ell0=28.741711216374707, sigma_f0=0.21305261382994262, ell1=0.90717603784446266)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hamming SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -34,179 +114,83 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.43216924708580134, sigma_f=0.75326118251964591, ell=11.123560434547556)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>52Structure</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=9.9999999999544897e-06)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=7.1857373549553616)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Predicted?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Saved?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>In progress</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEHamming 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>kernel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_ML</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOO_log_P</t>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.36174810262344692, ell=16.976484047437637)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.38187830426922176, ell0=783.32684463439443, ell1=15.804026532359993)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -403,43 +387,31 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Hypers(var_n=0.33623853006661136, ell=32.060321150982823)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35483375851541427, sigma_f=0.93171412929598607, ell=21.939841462467648)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35945193551611304, ell0=39.160914149618925, ell1=56.429026505115033)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.30307552926252879, ell0=28.741711216374707, sigma_f0=0.21305261382994262, ell1=0.90717603784446266)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hamming SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
+    <t>Hypers(ell=12.382259384067231)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -447,123 +419,155 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.43216924708580134, sigma_f=0.75326118251964591, ell=11.123560434547556)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.36174810262344692, ell=16.976484047437637)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.38187830426922176, ell0=783.32684463439443, ell1=15.804026532359993)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure SEHamming</t>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=9.9999999999544897e-06)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=7.1857373549553616)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Predicted?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saved?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEHamming 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_ML</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOO_log_P</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -571,12 +575,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -956,8 +954,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -967,42 +965,42 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2">
         <v>-104.296829</v>
@@ -1011,21 +1009,21 @@
         <v>0.99829999999999997</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2">
         <v>-107.403991</v>
@@ -1034,21 +1032,21 @@
         <v>0.98550000000000004</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C4" s="2">
         <v>-109.175516</v>
@@ -1057,21 +1055,21 @@
         <v>0.96719999999999995</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>-109.63411600000001</v>
@@ -1080,21 +1078,21 @@
         <v>0.97330000000000005</v>
       </c>
       <c r="H5" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1">
         <v>-115.755686</v>
@@ -1103,21 +1101,21 @@
         <v>0.5242</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>-90.516735999999995</v>
@@ -1126,21 +1124,21 @@
         <v>0.99429999999999996</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8">
         <v>-95.730936999999997</v>
@@ -1149,21 +1147,21 @@
         <v>0.95009999999999994</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>-96.168786999999995</v>
@@ -1172,21 +1170,21 @@
         <v>0.95469999999999999</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>-99.691761999999997</v>
@@ -1195,21 +1193,21 @@
         <v>0.86580000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="C11" s="2">
         <v>-85.655743000000001</v>
@@ -1218,21 +1216,21 @@
         <v>0.93230000000000002</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2">
         <v>-85.967275999999998</v>
@@ -1241,21 +1239,21 @@
         <v>0.96099999999999997</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2">
         <v>-90.150796</v>
@@ -1264,21 +1262,21 @@
         <v>0.94389999999999996</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <v>-93.403767999999999</v>
@@ -1287,21 +1285,21 @@
         <v>0.92789999999999995</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>-94.193860000000001</v>
@@ -1310,21 +1308,21 @@
         <v>0.93010000000000004</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J15" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C16">
         <v>-86.014349999999993</v>
@@ -1333,21 +1331,21 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>-95.681375000000003</v>
@@ -1356,21 +1354,21 @@
         <v>0.9768</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J17" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18">
         <v>-96.199038000000002</v>
@@ -1379,21 +1377,21 @@
         <v>0.98060000000000003</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>-100.18935999999999</v>
@@ -1402,21 +1400,21 @@
         <v>0.91359999999999997</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>-187.46480099999999</v>
@@ -1431,21 +1429,21 @@
         <v>0.45169999999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J20" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>-188.51542900000001</v>
@@ -1460,21 +1458,21 @@
         <v>0.46039999999999998</v>
       </c>
       <c r="H21" t="s">
-        <v>122</v>
+        <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>-188.611998</v>
@@ -1489,21 +1487,21 @@
         <v>0.45960000000000001</v>
       </c>
       <c r="H22" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J22" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>-189.126045</v>
@@ -1518,21 +1516,21 @@
         <v>0.4602</v>
       </c>
       <c r="H23" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>-204.32833099999999</v>
@@ -1547,21 +1545,21 @@
         <v>0.22839999999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="I24" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>-182.15376599999999</v>
@@ -1576,21 +1574,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="I25" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J25" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C26">
         <v>-182.15387799999999</v>
@@ -1605,21 +1603,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="I26" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1">
       <c r="A27" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2">
         <v>-182.15550500000001</v>
@@ -1634,21 +1632,21 @@
         <v>0.5161</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C28">
         <v>-182.15568300000001</v>
@@ -1663,21 +1661,21 @@
         <v>0.5161</v>
       </c>
       <c r="H28" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="I28" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J28" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C29">
         <v>-182.38603000000001</v>
@@ -1692,21 +1690,21 @@
         <v>0.51190000000000002</v>
       </c>
       <c r="H29" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="I29" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J29" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <v>-182.52230900000001</v>
@@ -1721,21 +1719,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I30" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J30" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C31">
         <v>-182.52231499999999</v>
@@ -1750,21 +1748,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J31" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C32">
         <v>-203.77469500000001</v>
@@ -1779,21 +1777,21 @@
         <v>0.35139999999999999</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I32" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J32" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2">
         <v>-149.854615</v>
@@ -1808,21 +1806,21 @@
         <v>0.57420000000000004</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>-150.395522</v>
@@ -1837,21 +1835,21 @@
         <v>0.57089999999999996</v>
       </c>
       <c r="H34" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="I34" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J34" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>-150.76389699999999</v>
@@ -1866,21 +1864,21 @@
         <v>0.5696</v>
       </c>
       <c r="H35" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="I35" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J35" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2">
         <v>-150.853938</v>
@@ -1895,21 +1893,21 @@
         <v>0.56789999999999996</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>-151.265311</v>
@@ -1924,21 +1922,21 @@
         <v>0.56659999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="I37" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J37" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>-166.89236399999999</v>
@@ -1953,21 +1951,21 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="I38" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J38" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>-167.263352</v>
@@ -1982,21 +1980,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H39" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="I39" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J39" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C40">
         <v>-167.263441</v>
@@ -2011,21 +2009,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H40" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I40" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J40" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C41">
         <v>-167.358092</v>
@@ -2040,21 +2038,21 @@
         <v>0.56479999999999997</v>
       </c>
       <c r="H41" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I41" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J41" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C42">
         <v>-167.47835000000001</v>
@@ -2069,21 +2067,21 @@
         <v>0.56850000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="I42" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J42" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C43">
         <v>-167.644937</v>
@@ -2098,21 +2096,21 @@
         <v>0.56569999999999998</v>
       </c>
       <c r="H43" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="I43" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J43" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C44">
         <v>-167.81095999999999</v>
@@ -2127,21 +2125,21 @@
         <v>0.56979999999999997</v>
       </c>
       <c r="H44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I44" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J44" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="C45">
         <v>-168.47959399999999</v>
@@ -2156,21 +2154,21 @@
         <v>0.55820000000000003</v>
       </c>
       <c r="H45" t="s">
-        <v>132</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J45" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="C46">
         <v>-192.916416</v>
@@ -2185,21 +2183,21 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>124</v>
+        <v>37</v>
       </c>
       <c r="I46" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J46" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="C47">
         <v>-193.712221</v>
@@ -2214,21 +2212,21 @@
         <v>0.45739999999999997</v>
       </c>
       <c r="H47" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="I47" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J47" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>-193.892056</v>
@@ -2243,21 +2241,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H48" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="I48" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J48" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="C49">
         <v>-194.433592</v>
@@ -2272,21 +2270,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="I49" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J49" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C50">
         <v>-207.70643999999999</v>
@@ -2301,24 +2299,22 @@
         <v>0.18859999999999999</v>
       </c>
       <c r="H50" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I50" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="J50" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="B3:B1048576"/>
     <sortCondition descending="1" ref="C3:C1048576"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2340,36 +2336,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>-148.93375</v>
@@ -2384,11 +2380,10 @@
         <v>0.57379999999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Fix headers on binary predictions. Update models.xlsx
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -20,21 +20,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="135">
-  <si>
-    <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure SEHamming</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="136">
+  <si>
+    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEHamming 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_ML</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOO_log_P</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -42,131 +58,179 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Hypers(var_n=0.18673420272755697, ell0=184.17411469863069, ell1=14.14952382022827, var_p0=1.0000000000000001e-05)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.18655586807239488, ell0=184.48405585006759, ell1=14.145790499076451)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.34846026420753662, ell=28.741286142106219)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell=12.382259384067231)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_GFP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=9.9999999999544897e-06)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bin_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_p=7.1857373549553616)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32Structure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Predicted?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saved?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Yes</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Hypers(var_n=0.33623853006661136, ell=32.060321150982823)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35483375851541427, sigma_f=0.93171412929598607, ell=21.939841462467648)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure 32Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35945193551611304, ell0=39.160914149618925, ell1=56.429026505115033)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.30307552926252879, ell0=28.741711216374707, sigma_f0=0.21305261382994262, ell1=0.90717603784446266)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hamming SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">52Structure </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intensity_ratio</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum_ratio</t>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_gfp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure 52Structure structure</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -363,15 +427,119 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Hypers(var_n=0.18673420272755697, ell0=184.17411469863069, ell1=14.14952382022827, var_p0=1.0000000000000001e-05)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.18655586807239488, ell0=184.48405585006759, ell1=14.145790499076451)</t>
+    <t xml:space="preserve">52Structure 32Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=1.0000000000000001e-05, var_p0=0.89487724953915782, sigma_f0=0.66984160463720055, ell0=1.9025628162948289)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure SEHamming</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.33623853006661136, ell=32.060321150982823)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35483375851541427, sigma_f=0.93171412929598607, ell=21.939841462467648)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">52Structure 32Structure </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35945193551611304, ell0=39.160914149618925, ell1=56.429026505115033)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>52Structure SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.30307552926252879, ell0=28.741711216374707, sigma_f0=0.21305261382994262, ell1=0.90717603784446266)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hamming SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKate_mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.36328578324159122, ell0=17.106511789569627, ell1=1682.3416381508896)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.40030811970907682, sigma_f=0.74115837975855214, ell=11.512595805037753)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEStructure</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.28201379709543717, sigma_f=1.0966688385241639, ell=28.33087986436426)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>log_mKate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.24957715479946413, ell=33.863661076974068)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.27282404881826822, ell0=43.287755987849479, ell1=56.956160231716908)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.35977555005130146, ell=16.731116127141021)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -379,195 +547,31 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>mKate_mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.34846026420753662, ell=28.741286142106219)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell=12.382259384067231)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.19314878348622011, ell=14.279062531880648)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1884561997177694, ell=13.664097736017478)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=14.274052420267843, ell1=12.607273199522607)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_GFP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=9.9999999999544897e-06)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bin_mKate</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_p=7.1857373549553616)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(ell0=21.374063357715098, ell1=19.58565740046425)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Predicted?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Saved?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(sigma_f=3.1780037828808068, ell=24.682249776102857)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.31797527958628913, var_p=0.78298570258561351)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.26445069144318911, ell=30.663467125258983)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_gfp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.23154340038876808, sigma_f=0.98728818923958717, ell=12.971769719915816)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.1597365355798829, sigma_f0=0.18270652828736142, ell0=0.90426045706946279, ell1=14.279290215609198)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEStructure 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEHamming 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.18873978857477752, sigma_f0=0.054229955196518791, ell0=1.0000000000000001e-05, ell1=14.246306242373095, var_p0=0.017128904154708375)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>32Structure 52Structure structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>kernel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_ML</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOO_log_P</t>
+    <t>sum_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.38091393540638624, ell=15.71198200081867)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.80847396298900576, var_p=0.38491010506868734)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intensity_ratio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.34316631115526602, ell=18.231430042054754)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum_ratio</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -955,7 +959,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -965,42 +969,42 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="I1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2">
         <v>-104.296829</v>
@@ -1009,21 +1013,21 @@
         <v>0.99829999999999997</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>-107.403991</v>
@@ -1032,21 +1036,21 @@
         <v>0.98550000000000004</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2">
         <v>-109.175516</v>
@@ -1055,21 +1059,21 @@
         <v>0.96719999999999995</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>112</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>-109.63411600000001</v>
@@ -1078,21 +1082,21 @@
         <v>0.97330000000000005</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>-115.755686</v>
@@ -1101,21 +1105,21 @@
         <v>0.5242</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>-90.516735999999995</v>
@@ -1124,21 +1128,21 @@
         <v>0.99429999999999996</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <v>-95.730936999999997</v>
@@ -1147,21 +1151,21 @@
         <v>0.95009999999999994</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C9">
         <v>-96.168786999999995</v>
@@ -1170,21 +1174,21 @@
         <v>0.95469999999999999</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>-99.691761999999997</v>
@@ -1193,21 +1197,21 @@
         <v>0.86580000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="I10" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1">
       <c r="A11" s="2" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
         <v>-85.655743000000001</v>
@@ -1216,21 +1220,21 @@
         <v>0.93230000000000002</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
         <v>-85.967275999999998</v>
@@ -1239,21 +1243,21 @@
         <v>0.96099999999999997</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>112</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>-90.150796</v>
@@ -1262,21 +1266,21 @@
         <v>0.94389999999999996</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C14">
         <v>-93.403767999999999</v>
@@ -1285,21 +1289,21 @@
         <v>0.92789999999999995</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>-94.193860000000001</v>
@@ -1308,21 +1312,21 @@
         <v>0.93010000000000004</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C16">
         <v>-86.014349999999993</v>
@@ -1331,21 +1335,21 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="I16" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C17">
         <v>-95.681375000000003</v>
@@ -1354,21 +1358,21 @@
         <v>0.9768</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J17" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C18">
         <v>-96.199038000000002</v>
@@ -1377,21 +1381,21 @@
         <v>0.98060000000000003</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J18" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C19">
         <v>-100.18935999999999</v>
@@ -1400,21 +1404,21 @@
         <v>0.91359999999999997</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J19" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="C20">
         <v>-187.46480099999999</v>
@@ -1429,21 +1433,21 @@
         <v>0.45169999999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="I20" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="C21">
         <v>-188.51542900000001</v>
@@ -1458,21 +1462,21 @@
         <v>0.46039999999999998</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="I21" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J21" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>-188.611998</v>
@@ -1487,21 +1491,21 @@
         <v>0.45960000000000001</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J22" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C23">
         <v>-189.126045</v>
@@ -1516,21 +1520,21 @@
         <v>0.4602</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J23" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="C24">
         <v>-204.32833099999999</v>
@@ -1545,21 +1549,21 @@
         <v>0.22839999999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J24" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C25">
         <v>-182.15376599999999</v>
@@ -1574,21 +1578,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J25" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C26">
         <v>-182.15387799999999</v>
@@ -1603,21 +1607,21 @@
         <v>0.51719999999999999</v>
       </c>
       <c r="H26" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J26" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1">
       <c r="A27" s="2" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2">
         <v>-182.15550500000001</v>
@@ -1632,21 +1636,21 @@
         <v>0.5161</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C28">
         <v>-182.15568300000001</v>
@@ -1661,21 +1665,21 @@
         <v>0.5161</v>
       </c>
       <c r="H28" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="I28" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J28" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="C29">
         <v>-182.38603000000001</v>
@@ -1690,21 +1694,21 @@
         <v>0.51190000000000002</v>
       </c>
       <c r="H29" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J29" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C30">
         <v>-182.52230900000001</v>
@@ -1719,21 +1723,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H30" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="I30" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J30" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C31">
         <v>-182.52231499999999</v>
@@ -1748,21 +1752,21 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="I31" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J31" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C32">
         <v>-203.77469500000001</v>
@@ -1777,21 +1781,21 @@
         <v>0.35139999999999999</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="I32" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J32" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2">
         <v>-149.854615</v>
@@ -1806,21 +1810,21 @@
         <v>0.57420000000000004</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="C34">
         <v>-150.395522</v>
@@ -1835,21 +1839,21 @@
         <v>0.57089999999999996</v>
       </c>
       <c r="H34" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="I34" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J34" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C35">
         <v>-150.76389699999999</v>
@@ -1864,21 +1868,21 @@
         <v>0.5696</v>
       </c>
       <c r="H35" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="I35" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J35" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="C36" s="2">
         <v>-150.853938</v>
@@ -1893,21 +1897,21 @@
         <v>0.56789999999999996</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="C37">
         <v>-151.265311</v>
@@ -1922,21 +1926,21 @@
         <v>0.56659999999999999</v>
       </c>
       <c r="H37" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="I37" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J37" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C38">
         <v>-166.89236399999999</v>
@@ -1951,21 +1955,21 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="I38" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J38" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="C39">
         <v>-167.263352</v>
@@ -1980,21 +1984,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H39" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="I39" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J39" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="C40">
         <v>-167.263441</v>
@@ -2009,21 +2013,21 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H40" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J40" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C41">
         <v>-167.358092</v>
@@ -2038,21 +2042,21 @@
         <v>0.56479999999999997</v>
       </c>
       <c r="H41" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="I41" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J41" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C42">
         <v>-167.47835000000001</v>
@@ -2067,21 +2071,21 @@
         <v>0.56850000000000001</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="I42" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J42" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="C43">
         <v>-167.644937</v>
@@ -2096,21 +2100,21 @@
         <v>0.56569999999999998</v>
       </c>
       <c r="H43" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="I43" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J43" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C44">
         <v>-167.81095999999999</v>
@@ -2125,21 +2129,21 @@
         <v>0.56979999999999997</v>
       </c>
       <c r="H44" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="I44" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J44" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="C45">
         <v>-168.47959399999999</v>
@@ -2154,21 +2158,21 @@
         <v>0.55820000000000003</v>
       </c>
       <c r="H45" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="I45" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J45" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="C46">
         <v>-192.916416</v>
@@ -2183,21 +2187,21 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="I46" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J46" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="C47">
         <v>-193.712221</v>
@@ -2212,21 +2216,21 @@
         <v>0.45739999999999997</v>
       </c>
       <c r="H47" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="I47" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J47" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>129</v>
       </c>
       <c r="C48">
         <v>-193.892056</v>
@@ -2241,21 +2245,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H48" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="I48" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J48" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C49">
         <v>-194.433592</v>
@@ -2270,21 +2274,21 @@
         <v>0.45800000000000002</v>
       </c>
       <c r="H49" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I49" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J49" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C50">
         <v>-207.70643999999999</v>
@@ -2299,16 +2303,17 @@
         <v>0.18859999999999999</v>
       </c>
       <c r="H50" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="I50" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J50" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="B3:B1048576"/>
     <sortCondition descending="1" ref="C3:C1048576"/>
@@ -2336,36 +2341,36 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C2">
         <v>-148.93375</v>
@@ -2380,10 +2385,11 @@
         <v>0.57379999999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update models.xlsx to reflect predictions for bin_intensity.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-23980" yWindow="740" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="-23900" yWindow="820" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
   <si>
     <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -574,12 +574,18 @@
     <t>sum_ratio</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -631,7 +637,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -954,15 +960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
@@ -1114,27 +1119,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" s="2" customFormat="1">
+      <c r="A7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>-90.516735999999995</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.99429999999999996</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
+      <c r="I7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2313,7 +2318,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD1048576">
     <sortCondition ref="B3:B1048576"/>
     <sortCondition descending="1" ref="C3:C1048576"/>
@@ -2321,7 +2325,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2329,15 +2333,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -2389,12 +2392,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Add E-phys data and some models.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -10,7 +10,7 @@
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="train" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="137">
   <si>
     <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -576,9 +576,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -964,7 +961,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1136,7 +1133,7 @@
         <v>98</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>136</v>
@@ -1326,27 +1323,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" s="2" customFormat="1">
+      <c r="A16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>-86.014349999999993</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.99980000000000002</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" t="s">
-        <v>39</v>
+      <c r="I16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:10">

</xml_diff>

<commit_message>
Try some models for e-phys data.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-23900" yWindow="820" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="1700" yWindow="0" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
   <si>
     <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -577,12 +577,48 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>hamming</t>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.33746585170295385, var_p=0.90462297543234549)</t>
+  </si>
+  <si>
+    <t>log_mKate</t>
+  </si>
+  <si>
+    <t>32Hamming</t>
+  </si>
+  <si>
+    <t>52Hamming</t>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.25945513823855021, ell=13.719587674232427)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEHamming </t>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.27334001654923046, ell=12.319384895174005)</t>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.28499045030012438, sigma_f=0.94938874325886691, ell=9.7242866470916614)</t>
+  </si>
+  <si>
+    <t>32Structure</t>
+  </si>
+  <si>
+    <t>log_gfp</t>
+  </si>
+  <si>
+    <t>Hypers(var_n=0.1652602162827384, ell=14.850275270523646)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -604,6 +640,18 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -622,15 +670,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,15 +1018,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1823,112 +1884,97 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C34">
-        <v>-150.395522</v>
+        <v>-149.96259800000001</v>
       </c>
       <c r="D34">
-        <v>-139.471025</v>
+        <v>-139.93741299999999</v>
       </c>
       <c r="E34">
-        <v>0.77910000000000001</v>
+        <v>0.77680000000000005</v>
       </c>
       <c r="F34">
-        <v>0.57089999999999996</v>
+        <v>0.56169999999999998</v>
       </c>
       <c r="H34" t="s">
-        <v>122</v>
-      </c>
-      <c r="I34" t="s">
-        <v>39</v>
-      </c>
-      <c r="J34" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="C35">
-        <v>-150.76389699999999</v>
+        <v>-150.23073099999999</v>
       </c>
       <c r="D35">
-        <v>-139.48403099999999</v>
+        <v>-140.80470800000001</v>
       </c>
       <c r="E35">
-        <v>0.77929999999999999</v>
+        <v>0.77439999999999998</v>
       </c>
       <c r="F35">
-        <v>0.5696</v>
+        <v>0.56210000000000004</v>
       </c>
       <c r="H35" t="s">
-        <v>125</v>
-      </c>
-      <c r="I35" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1">
-      <c r="A36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="2">
-        <v>-150.853938</v>
-      </c>
-      <c r="D36" s="2">
-        <v>-139.5686</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0.77990000000000004</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0.56789999999999996</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36">
+        <v>-150.25345899999999</v>
+      </c>
+      <c r="D36">
+        <v>-139.86114900000001</v>
+      </c>
+      <c r="E36">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="F36">
+        <v>0.56110000000000004</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I36"/>
+      <c r="J36"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C37">
-        <v>-151.265311</v>
+        <v>-150.395522</v>
       </c>
       <c r="D37">
-        <v>-139.80320699999999</v>
+        <v>-139.471025</v>
       </c>
       <c r="E37">
-        <v>0.77980000000000005</v>
+        <v>0.77910000000000001</v>
       </c>
       <c r="F37">
-        <v>0.56659999999999999</v>
+        <v>0.57089999999999996</v>
       </c>
       <c r="H37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I37" t="s">
         <v>39</v>
@@ -1939,54 +1985,48 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C38">
-        <v>-166.89236399999999</v>
+        <v>-150.604209</v>
       </c>
       <c r="D38">
-        <v>-156.14573999999999</v>
+        <v>-140.00274099999999</v>
       </c>
       <c r="E38">
-        <v>0.7218</v>
+        <v>0.77749999999999997</v>
       </c>
       <c r="F38">
-        <v>0.56999999999999995</v>
+        <v>0.56089999999999995</v>
       </c>
       <c r="H38" t="s">
-        <v>107</v>
-      </c>
-      <c r="I38" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="C39">
-        <v>-167.263352</v>
+        <v>-150.76389699999999</v>
       </c>
       <c r="D39">
-        <v>-156.40886699999999</v>
+        <v>-139.48403099999999</v>
       </c>
       <c r="E39">
-        <v>0.72089999999999999</v>
+        <v>0.77929999999999999</v>
       </c>
       <c r="F39">
-        <v>0.56869999999999998</v>
+        <v>0.5696</v>
       </c>
       <c r="H39" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="I39" t="s">
         <v>39</v>
@@ -1996,55 +2036,56 @@
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40">
-        <v>-167.263441</v>
-      </c>
-      <c r="D40">
-        <v>-156.40904800000001</v>
-      </c>
-      <c r="E40">
-        <v>0.72089999999999999</v>
-      </c>
-      <c r="F40">
-        <v>0.56869999999999998</v>
-      </c>
-      <c r="H40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" t="s">
-        <v>39</v>
-      </c>
-      <c r="J40" t="s">
-        <v>39</v>
+      <c r="A40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="2">
+        <v>-150.853938</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-139.5686</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.56789999999999996</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
       <c r="C41">
-        <v>-167.358092</v>
+        <v>-151.265311</v>
       </c>
       <c r="D41">
-        <v>-157.24802399999999</v>
+        <v>-139.80320699999999</v>
       </c>
       <c r="E41">
-        <v>0.71619999999999995</v>
+        <v>0.77980000000000005</v>
       </c>
       <c r="F41">
-        <v>0.56479999999999997</v>
+        <v>0.56659999999999999</v>
       </c>
       <c r="H41" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="I41" t="s">
         <v>39</v>
@@ -2055,25 +2096,25 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C42">
-        <v>-167.47835000000001</v>
+        <v>-166.89236399999999</v>
       </c>
       <c r="D42">
-        <v>-156.46872099999999</v>
+        <v>-156.14573999999999</v>
       </c>
       <c r="E42">
-        <v>0.71930000000000005</v>
+        <v>0.7218</v>
       </c>
       <c r="F42">
-        <v>0.56850000000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I42" t="s">
         <v>39</v>
@@ -2084,25 +2125,25 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="C43">
-        <v>-167.644937</v>
+        <v>-167.263352</v>
       </c>
       <c r="D43">
-        <v>-156.811646</v>
+        <v>-156.40886699999999</v>
       </c>
       <c r="E43">
-        <v>0.71960000000000002</v>
+        <v>0.72089999999999999</v>
       </c>
       <c r="F43">
-        <v>0.56569999999999998</v>
+        <v>0.56869999999999998</v>
       </c>
       <c r="H43" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="I43" t="s">
         <v>39</v>
@@ -2113,25 +2154,25 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>-167.81095999999999</v>
+        <v>-167.263441</v>
       </c>
       <c r="D44">
-        <v>-158.146782</v>
+        <v>-156.40904800000001</v>
       </c>
       <c r="E44">
-        <v>0.70850000000000002</v>
+        <v>0.72089999999999999</v>
       </c>
       <c r="F44">
-        <v>0.56979999999999997</v>
+        <v>0.56869999999999998</v>
       </c>
       <c r="H44" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="I44" t="s">
         <v>39</v>
@@ -2142,25 +2183,25 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="C45">
-        <v>-168.47959399999999</v>
+        <v>-167.358092</v>
       </c>
       <c r="D45">
-        <v>-159.59816799999999</v>
+        <v>-157.24802399999999</v>
       </c>
       <c r="E45">
-        <v>0.70020000000000004</v>
+        <v>0.71619999999999995</v>
       </c>
       <c r="F45">
-        <v>0.55820000000000003</v>
+        <v>0.56479999999999997</v>
       </c>
       <c r="H45" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="I45" t="s">
         <v>39</v>
@@ -2171,25 +2212,25 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="C46">
-        <v>-192.916416</v>
+        <v>-167.47835000000001</v>
       </c>
       <c r="D46">
-        <v>-180.76219</v>
+        <v>-156.46872099999999</v>
       </c>
       <c r="E46">
-        <v>0.63919999999999999</v>
+        <v>0.71930000000000005</v>
       </c>
       <c r="F46">
-        <v>0.44700000000000001</v>
+        <v>0.56850000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="I46" t="s">
         <v>39</v>
@@ -2203,22 +2244,22 @@
         <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="C47">
-        <v>-193.712221</v>
+        <v>-167.644937</v>
       </c>
       <c r="D47">
-        <v>-190.48987</v>
+        <v>-156.811646</v>
       </c>
       <c r="E47">
-        <v>0.64290000000000003</v>
+        <v>0.71960000000000002</v>
       </c>
       <c r="F47">
-        <v>0.45739999999999997</v>
+        <v>0.56569999999999998</v>
       </c>
       <c r="H47" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="I47" t="s">
         <v>39</v>
@@ -2229,25 +2270,25 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="C48">
-        <v>-193.892056</v>
+        <v>-167.81095999999999</v>
       </c>
       <c r="D48">
-        <v>-180.553665</v>
+        <v>-158.146782</v>
       </c>
       <c r="E48">
-        <v>0.64359999999999995</v>
+        <v>0.70850000000000002</v>
       </c>
       <c r="F48">
-        <v>0.45800000000000002</v>
+        <v>0.56979999999999997</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="I48" t="s">
         <v>39</v>
@@ -2258,25 +2299,25 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="C49">
-        <v>-194.433592</v>
+        <v>-168.47959399999999</v>
       </c>
       <c r="D49">
-        <v>-180.39733799999999</v>
+        <v>-159.59816799999999</v>
       </c>
       <c r="E49">
-        <v>0.64400000000000002</v>
+        <v>0.70020000000000004</v>
       </c>
       <c r="F49">
-        <v>0.45800000000000002</v>
+        <v>0.55820000000000003</v>
       </c>
       <c r="H49" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="I49" t="s">
         <v>39</v>
@@ -2287,40 +2328,180 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50">
+        <v>-192.916416</v>
+      </c>
+      <c r="D50">
+        <v>-180.76219</v>
+      </c>
+      <c r="E50">
+        <v>0.63919999999999999</v>
+      </c>
+      <c r="F50">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="H50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I50" t="s">
+        <v>39</v>
+      </c>
+      <c r="J50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51">
+        <v>-193.712221</v>
+      </c>
+      <c r="D51">
+        <v>-190.48987</v>
+      </c>
+      <c r="E51">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="F51">
+        <v>0.45739999999999997</v>
+      </c>
+      <c r="H51" t="s">
+        <v>127</v>
+      </c>
+      <c r="I51" t="s">
+        <v>39</v>
+      </c>
+      <c r="J51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52">
+        <v>-193.892056</v>
+      </c>
+      <c r="D52">
+        <v>-180.553665</v>
+      </c>
+      <c r="E52">
+        <v>0.64359999999999995</v>
+      </c>
+      <c r="F52">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="H52" t="s">
+        <v>130</v>
+      </c>
+      <c r="I52" t="s">
+        <v>39</v>
+      </c>
+      <c r="J52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53">
+        <v>-194.433592</v>
+      </c>
+      <c r="D53">
+        <v>-180.39733799999999</v>
+      </c>
+      <c r="E53">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="F53">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="H53" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" t="s">
+        <v>39</v>
+      </c>
+      <c r="J53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
         <v>69</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B54" t="s">
         <v>70</v>
       </c>
-      <c r="C50">
+      <c r="C54">
         <v>-207.70643999999999</v>
       </c>
-      <c r="D50">
+      <c r="D54">
         <v>-203.65018900000001</v>
       </c>
-      <c r="E50">
+      <c r="E54">
         <v>0.29559999999999997</v>
       </c>
-      <c r="F50">
+      <c r="F54">
         <v>0.18859999999999999</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H54" t="s">
         <v>71</v>
       </c>
-      <c r="I50" t="s">
-        <v>39</v>
-      </c>
-      <c r="J50" t="s">
-        <v>39</v>
+      <c r="I54" t="s">
+        <v>39</v>
+      </c>
+      <c r="J54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55">
+        <v>-182.26541399999999</v>
+      </c>
+      <c r="D55">
+        <v>-164.74364399999999</v>
+      </c>
+      <c r="E55">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="F55">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="H55" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD1048576">
-    <sortCondition ref="B3:B1048576"/>
-    <sortCondition descending="1" ref="C3:C1048576"/>
+  <sortState ref="A2:J54">
+    <sortCondition ref="B2:B54"/>
+    <sortCondition descending="1" ref="C2:C54"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Try bin_mKate with 0s dropped.
</commit_message>
<xml_diff>
--- a/2016-02-17_data/models.xlsx
+++ b/2016-02-17_data/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="0" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="-25480" yWindow="1220" windowWidth="25160" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="150">
   <si>
     <t>Hypers(var_n=0.17221138236080849, sigma_f0=0.13952844989470831, ell0=0.90852288508627521, ell1=14.246519289116554, var_p0=0.017125767238569151)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>Hypers(var_n=0.1652602162827384, ell=14.850275270523646)</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -670,8 +673,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -684,13 +747,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1739,54 +1862,48 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="C29">
-        <v>-182.38603000000001</v>
+        <v>-182.26541399999999</v>
       </c>
       <c r="D29">
-        <v>-165.07706400000001</v>
+        <v>-164.74364399999999</v>
       </c>
       <c r="E29">
-        <v>0.69789999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="F29">
-        <v>0.51190000000000002</v>
+        <v>0.51570000000000005</v>
       </c>
       <c r="H29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I29" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C30">
-        <v>-182.52230900000001</v>
+        <v>-182.38603000000001</v>
       </c>
       <c r="D30">
-        <v>-164.318455</v>
+        <v>-165.07706400000001</v>
       </c>
       <c r="E30">
-        <v>0.70140000000000002</v>
+        <v>0.69789999999999996</v>
       </c>
       <c r="F30">
-        <v>0.51900000000000002</v>
+        <v>0.51190000000000002</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="I30" t="s">
         <v>39</v>
@@ -1797,16 +1914,16 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
       </c>
       <c r="C31">
-        <v>-182.52231499999999</v>
+        <v>-182.52230900000001</v>
       </c>
       <c r="D31">
-        <v>-164.31815399999999</v>
+        <v>-164.318455</v>
       </c>
       <c r="E31">
         <v>0.70140000000000002</v>
@@ -1815,7 +1932,7 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="H31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I31" t="s">
         <v>39</v>
@@ -1826,324 +1943,332 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>65</v>
       </c>
       <c r="C32">
+        <v>-182.52231499999999</v>
+      </c>
+      <c r="D32">
+        <v>-164.31815399999999</v>
+      </c>
+      <c r="E32">
+        <v>0.70140000000000002</v>
+      </c>
+      <c r="F32">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33">
         <v>-203.77469500000001</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>-189.572025</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>0.48949999999999999</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>0.35139999999999999</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G33"/>
+      <c r="H33" t="s">
         <v>66</v>
       </c>
-      <c r="I32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="2" customFormat="1">
-      <c r="A33" s="2" t="s">
+      <c r="I33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>-149.854615</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <v>-139.42251999999999</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E34" s="2">
         <v>0.77890000000000004</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F34" s="2">
         <v>0.57420000000000004</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34">
-        <v>-149.96259800000001</v>
-      </c>
-      <c r="D34">
-        <v>-139.93741299999999</v>
-      </c>
-      <c r="E34">
-        <v>0.77680000000000005</v>
-      </c>
-      <c r="F34">
-        <v>0.56169999999999998</v>
-      </c>
-      <c r="H34" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
         <v>139</v>
       </c>
       <c r="C35">
-        <v>-150.23073099999999</v>
+        <v>-149.96259800000001</v>
       </c>
       <c r="D35">
-        <v>-140.80470800000001</v>
+        <v>-139.93741299999999</v>
       </c>
       <c r="E35">
-        <v>0.77439999999999998</v>
+        <v>0.77680000000000005</v>
       </c>
       <c r="F35">
-        <v>0.56210000000000004</v>
+        <v>0.56169999999999998</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="2" customFormat="1">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>139</v>
       </c>
       <c r="C36">
-        <v>-150.25345899999999</v>
+        <v>-150.23073099999999</v>
       </c>
       <c r="D36">
-        <v>-139.86114900000001</v>
+        <v>-140.80470800000001</v>
       </c>
       <c r="E36">
-        <v>0.77749999999999997</v>
+        <v>0.77439999999999998</v>
       </c>
       <c r="F36">
-        <v>0.56110000000000004</v>
+        <v>0.56210000000000004</v>
       </c>
       <c r="G36"/>
       <c r="H36" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I36"/>
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C37">
-        <v>-150.395522</v>
+        <v>-150.25345899999999</v>
       </c>
       <c r="D37">
-        <v>-139.471025</v>
+        <v>-139.86114900000001</v>
       </c>
       <c r="E37">
-        <v>0.77910000000000001</v>
+        <v>0.77749999999999997</v>
       </c>
       <c r="F37">
-        <v>0.57089999999999996</v>
+        <v>0.56110000000000004</v>
       </c>
       <c r="H37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="J37" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C38">
-        <v>-150.604209</v>
+        <v>-150.395522</v>
       </c>
       <c r="D38">
-        <v>-140.00274099999999</v>
+        <v>-139.471025</v>
       </c>
       <c r="E38">
-        <v>0.77749999999999997</v>
+        <v>0.77910000000000001</v>
       </c>
       <c r="F38">
-        <v>0.56089999999999995</v>
+        <v>0.57089999999999996</v>
       </c>
       <c r="H38" t="s">
-        <v>142</v>
+        <v>122</v>
+      </c>
+      <c r="I38" t="s">
+        <v>136</v>
+      </c>
+      <c r="J38" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39">
+        <v>-150.604209</v>
+      </c>
+      <c r="D39">
+        <v>-140.00274099999999</v>
+      </c>
+      <c r="E39">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="F39">
+        <v>0.56089999999999995</v>
+      </c>
+      <c r="H39" t="s">
+        <v>142</v>
+      </c>
+      <c r="J39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
         <v>108</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>-150.76389699999999</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>-139.48403099999999</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>0.77929999999999999</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>0.5696</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>125</v>
       </c>
-      <c r="I39" t="s">
-        <v>39</v>
-      </c>
-      <c r="J39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="2" t="s">
+      <c r="I40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C41" s="2">
         <v>-150.853938</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D41" s="2">
         <v>-139.5686</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E41" s="2">
         <v>0.77990000000000004</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F41" s="2">
         <v>0.56789999999999996</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41">
-        <v>-151.265311</v>
-      </c>
-      <c r="D41">
-        <v>-139.80320699999999</v>
-      </c>
-      <c r="E41">
-        <v>0.77980000000000005</v>
-      </c>
-      <c r="F41">
-        <v>0.56659999999999999</v>
-      </c>
-      <c r="H41" t="s">
-        <v>124</v>
-      </c>
-      <c r="I41" t="s">
-        <v>39</v>
-      </c>
-      <c r="J41" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C42">
-        <v>-166.89236399999999</v>
+        <v>-151.265311</v>
       </c>
       <c r="D42">
-        <v>-156.14573999999999</v>
+        <v>-139.80320699999999</v>
       </c>
       <c r="E42">
-        <v>0.7218</v>
+        <v>0.77980000000000005</v>
       </c>
       <c r="F42">
-        <v>0.56999999999999995</v>
+        <v>0.56659999999999999</v>
       </c>
       <c r="H42" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="I42" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C43">
-        <v>-167.263352</v>
+        <v>-166.89236399999999</v>
       </c>
       <c r="D43">
-        <v>-156.40886699999999</v>
+        <v>-156.14573999999999</v>
       </c>
       <c r="E43">
-        <v>0.72089999999999999</v>
+        <v>0.7218</v>
       </c>
       <c r="F43">
-        <v>0.56869999999999998</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H43" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I43" t="s">
         <v>39</v>
@@ -2154,16 +2279,16 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="C44">
-        <v>-167.263441</v>
+        <v>-167.263352</v>
       </c>
       <c r="D44">
-        <v>-156.40904800000001</v>
+        <v>-156.40886699999999</v>
       </c>
       <c r="E44">
         <v>0.72089999999999999</v>
@@ -2172,7 +2297,7 @@
         <v>0.56869999999999998</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="I44" t="s">
         <v>39</v>
@@ -2183,25 +2308,25 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <v>-167.358092</v>
+        <v>-167.263441</v>
       </c>
       <c r="D45">
-        <v>-157.24802399999999</v>
+        <v>-156.40904800000001</v>
       </c>
       <c r="E45">
-        <v>0.71619999999999995</v>
+        <v>0.72089999999999999</v>
       </c>
       <c r="F45">
-        <v>0.56479999999999997</v>
+        <v>0.56869999999999998</v>
       </c>
       <c r="H45" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="I45" t="s">
         <v>39</v>
@@ -2212,25 +2337,25 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
         <v>73</v>
       </c>
       <c r="C46">
-        <v>-167.47835000000001</v>
+        <v>-167.358092</v>
       </c>
       <c r="D46">
-        <v>-156.46872099999999</v>
+        <v>-157.24802399999999</v>
       </c>
       <c r="E46">
-        <v>0.71930000000000005</v>
+        <v>0.71619999999999995</v>
       </c>
       <c r="F46">
-        <v>0.56850000000000001</v>
+        <v>0.56479999999999997</v>
       </c>
       <c r="H46" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="I46" t="s">
         <v>39</v>
@@ -2241,25 +2366,25 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C47">
-        <v>-167.644937</v>
+        <v>-167.47835000000001</v>
       </c>
       <c r="D47">
-        <v>-156.811646</v>
+        <v>-156.46872099999999</v>
       </c>
       <c r="E47">
-        <v>0.71960000000000002</v>
+        <v>0.71930000000000005</v>
       </c>
       <c r="F47">
-        <v>0.56569999999999998</v>
+        <v>0.56850000000000001</v>
       </c>
       <c r="H47" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I47" t="s">
         <v>39</v>
@@ -2270,25 +2395,25 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>-167.81095999999999</v>
+        <v>-167.644937</v>
       </c>
       <c r="D48">
-        <v>-158.146782</v>
+        <v>-156.811646</v>
       </c>
       <c r="E48">
-        <v>0.70850000000000002</v>
+        <v>0.71960000000000002</v>
       </c>
       <c r="F48">
-        <v>0.56979999999999997</v>
+        <v>0.56569999999999998</v>
       </c>
       <c r="H48" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="I48" t="s">
         <v>39</v>
@@ -2299,25 +2424,25 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="C49">
-        <v>-168.47959399999999</v>
+        <v>-167.81095999999999</v>
       </c>
       <c r="D49">
-        <v>-159.59816799999999</v>
+        <v>-158.146782</v>
       </c>
       <c r="E49">
-        <v>0.70020000000000004</v>
+        <v>0.70850000000000002</v>
       </c>
       <c r="F49">
-        <v>0.55820000000000003</v>
+        <v>0.56979999999999997</v>
       </c>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I49" t="s">
         <v>39</v>
@@ -2328,25 +2453,25 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C50">
-        <v>-192.916416</v>
+        <v>-168.47959399999999</v>
       </c>
       <c r="D50">
-        <v>-180.76219</v>
+        <v>-159.59816799999999</v>
       </c>
       <c r="E50">
-        <v>0.63919999999999999</v>
+        <v>0.70020000000000004</v>
       </c>
       <c r="F50">
-        <v>0.44700000000000001</v>
+        <v>0.55820000000000003</v>
       </c>
       <c r="H50" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="I50" t="s">
         <v>39</v>
@@ -2357,25 +2482,25 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C51">
-        <v>-193.712221</v>
+        <v>-192.916416</v>
       </c>
       <c r="D51">
-        <v>-190.48987</v>
+        <v>-180.76219</v>
       </c>
       <c r="E51">
-        <v>0.64290000000000003</v>
+        <v>0.63919999999999999</v>
       </c>
       <c r="F51">
-        <v>0.45739999999999997</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="H51" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="I51" t="s">
         <v>39</v>
@@ -2386,25 +2511,25 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52">
-        <v>-193.892056</v>
+        <v>-193.712221</v>
       </c>
       <c r="D52">
-        <v>-180.553665</v>
+        <v>-190.48987</v>
       </c>
       <c r="E52">
-        <v>0.64359999999999995</v>
+        <v>0.64290000000000003</v>
       </c>
       <c r="F52">
-        <v>0.45800000000000002</v>
+        <v>0.45739999999999997</v>
       </c>
       <c r="H52" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I52" t="s">
         <v>39</v>
@@ -2415,25 +2540,25 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="C53">
-        <v>-194.433592</v>
+        <v>-193.892056</v>
       </c>
       <c r="D53">
-        <v>-180.39733799999999</v>
+        <v>-180.553665</v>
       </c>
       <c r="E53">
-        <v>0.64400000000000002</v>
+        <v>0.64359999999999995</v>
       </c>
       <c r="F53">
         <v>0.45800000000000002</v>
       </c>
       <c r="H53" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="I53" t="s">
         <v>39</v>
@@ -2444,25 +2569,25 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C54">
-        <v>-207.70643999999999</v>
+        <v>-194.433592</v>
       </c>
       <c r="D54">
-        <v>-203.65018900000001</v>
+        <v>-180.39733799999999</v>
       </c>
       <c r="E54">
-        <v>0.29559999999999997</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F54">
-        <v>0.18859999999999999</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="H54" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="I54" t="s">
         <v>39</v>
@@ -2473,31 +2598,37 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="C55">
-        <v>-182.26541399999999</v>
+        <v>-207.70643999999999</v>
       </c>
       <c r="D55">
-        <v>-164.74364399999999</v>
+        <v>-203.65018900000001</v>
       </c>
       <c r="E55">
-        <v>0.69899999999999995</v>
+        <v>0.29559999999999997</v>
       </c>
       <c r="F55">
-        <v>0.51570000000000005</v>
+        <v>0.18859999999999999</v>
       </c>
       <c r="H55" t="s">
-        <v>148</v>
+        <v>71</v>
+      </c>
+      <c r="I55" t="s">
+        <v>39</v>
+      </c>
+      <c r="J55" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J54">
-    <sortCondition ref="B2:B54"/>
-    <sortCondition descending="1" ref="C2:C54"/>
+  <sortState ref="A2:J56">
+    <sortCondition ref="B2:B56"/>
+    <sortCondition descending="1" ref="C2:C56"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>